<commit_message>
vivado loop pipelining report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/LoopPipeliningSolution/power/LoopPipeliningClockEnablePowerReport.xlsx
+++ b/reports/vivado/LoopPipeliningSolution/power/LoopPipeliningClockEnablePowerReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>Utilization</t>
   </si>
@@ -44,54 +44,54 @@
     <t/>
   </si>
   <si>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_30</t>
+  </si>
+  <si>
+    <t>myclk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF </t>
+  </si>
+  <si>
     <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_00</t>
   </si>
   <si>
-    <t>myclk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FF </t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_30</t>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_90</t>
+  </si>
+  <si>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_80</t>
+  </si>
+  <si>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_70</t>
   </si>
   <si>
     <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_40</t>
   </si>
   <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_70</t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_80</t>
-  </si>
-  <si>
     <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_10</t>
   </si>
   <si>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_50</t>
+  </si>
+  <si>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_20</t>
+  </si>
+  <si>
+    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_60</t>
+  </si>
+  <si>
+    <t>firConvolutionLoopPipelining_IP/U0/accumulator_reg_1140</t>
+  </si>
+  <si>
     <t>firConvolutionLoopPipelining_IP/U0/ap_NS_fsm1</t>
   </si>
   <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_20</t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_50</t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_60</t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/shiftRegister_90</t>
-  </si>
-  <si>
     <t>firConvolutionLoopPipelining_IP/U0/ap_enable_reg_pp0_iter2</t>
   </si>
   <si>
     <t xml:space="preserve">FF LUT </t>
   </si>
   <si>
-    <t>firConvolutionLoopPipelining_IP/U0/accumulator_reg_1140</t>
-  </si>
-  <si>
     <t>firConvolutionLoopPipelining_IP/U0/tmp_6_reg_463[16]_i_1_n_2</t>
   </si>
   <si>
@@ -101,22 +101,19 @@
     <t>firConvolutionLoopPipelining_IP/U0/ap_enable_reg_pp0_iter1</t>
   </si>
   <si>
+    <t>firConvolutionLoopPipelining_IP/U0/coefficientsFilter1_1_reg_4580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSP </t>
+  </si>
+  <si>
+    <t>firConvolutionLoopPipelining_IP/U0/ce0</t>
+  </si>
+  <si>
     <t>firConvolutionLoopPipelining_IP/U0/i_reg_1270</t>
   </si>
   <si>
     <t>firConvolutionLoopPipelining_IP/U0/tmp_4_reg_4300</t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/ce0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DSP </t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/coefficientsFilter1_1_reg_4580</t>
-  </si>
-  <si>
-    <t>firConvolutionLoopPipelining_IP/U0/ap_enable_reg_pp0_iter1_i_1_n_2</t>
   </si>
 </sst>
 </file>
@@ -238,7 +235,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>3.5073282197117805E-4</v>
+        <v>1.9623672415036708E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -264,22 +261,22 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>4.62653479189612E-5</v>
+        <v>2.8202610337757505E-5</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>33.4782600402832</v>
+        <v>33.043479919433594</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>5.349087238311768</v>
+        <v>5.609173774719238</v>
       </c>
       <c r="E3" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F3" t="n" s="7">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="G3" t="s" s="4">
         <v>11</v>
@@ -290,22 +287,22 @@
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>4.566450297716074E-5</v>
+        <v>2.6129782781936228E-5</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>13</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>33.043479919433594</v>
+        <v>33.4782600402832</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>5.609173774719238</v>
+        <v>5.349087238311768</v>
       </c>
       <c r="E4" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F4" t="n" s="7">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="G4" t="s" s="4">
         <v>11</v>
@@ -316,13 +313,13 @@
     </row>
     <row r="5" outlineLevel="1">
       <c r="A5" t="n" s="5">
-        <v>3.1244133424479514E-5</v>
+        <v>1.8403477952233516E-5</v>
       </c>
       <c r="B5" t="s" s="4">
         <v>14</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>22.60869598388672</v>
+        <v>11.30434799194336</v>
       </c>
       <c r="D5" t="n" s="2">
         <v>5.65217399597168</v>
@@ -331,7 +328,7 @@
         <v>32.0</v>
       </c>
       <c r="F5" t="n" s="7">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="G5" t="s" s="4">
         <v>11</v>
@@ -342,7 +339,7 @@
     </row>
     <row r="6" outlineLevel="1">
       <c r="A6" t="n" s="5">
-        <v>3.1244133424479514E-5</v>
+        <v>1.71486954059219E-5</v>
       </c>
       <c r="B6" t="s" s="4">
         <v>15</v>
@@ -357,7 +354,7 @@
         <v>32.0</v>
       </c>
       <c r="F6" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G6" t="s" s="4">
         <v>11</v>
@@ -368,7 +365,7 @@
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" t="n" s="5">
-        <v>3.1244133424479514E-5</v>
+        <v>1.3938260963186622E-5</v>
       </c>
       <c r="B7" t="s" s="4">
         <v>16</v>
@@ -383,7 +380,7 @@
         <v>32.0</v>
       </c>
       <c r="F7" t="n" s="7">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G7" t="s" s="4">
         <v>11</v>
@@ -394,22 +391,22 @@
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" t="n" s="5">
-        <v>3.064328484470025E-5</v>
+        <v>1.367826098430669E-5</v>
       </c>
       <c r="B8" t="s" s="4">
         <v>17</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>22.173913955688477</v>
+        <v>22.60869598388672</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>5.503129959106445</v>
+        <v>5.65217399597168</v>
       </c>
       <c r="E8" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F8" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G8" t="s" s="4">
         <v>11</v>
@@ -420,22 +417,22 @@
     </row>
     <row r="9" outlineLevel="1">
       <c r="A9" t="n" s="5">
-        <v>1.5622066712239757E-5</v>
+        <v>1.3093695997667965E-5</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>18</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>11.30434799194336</v>
+        <v>22.173913955688477</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>5.533477783203125</v>
+        <v>5.503129959106445</v>
       </c>
       <c r="E9" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F9" t="n" s="7">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="G9" t="s" s="4">
         <v>11</v>
@@ -446,7 +443,7 @@
     </row>
     <row r="10" outlineLevel="1">
       <c r="A10" t="n" s="5">
-        <v>1.5622066712239757E-5</v>
+        <v>1.0422609193483368E-5</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>19</v>
@@ -461,7 +458,7 @@
         <v>32.0</v>
       </c>
       <c r="F10" t="n" s="7">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="G10" t="s" s="4">
         <v>11</v>
@@ -472,7 +469,7 @@
     </row>
     <row r="11" outlineLevel="1">
       <c r="A11" t="n" s="5">
-        <v>1.5622066712239757E-5</v>
+        <v>7.986522177816369E-6</v>
       </c>
       <c r="B11" t="s" s="4">
         <v>20</v>
@@ -487,7 +484,7 @@
         <v>32.0</v>
       </c>
       <c r="F11" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G11" t="s" s="4">
         <v>11</v>
@@ -498,7 +495,7 @@
     </row>
     <row r="12" outlineLevel="1">
       <c r="A12" t="n" s="5">
-        <v>1.5622066712239757E-5</v>
+        <v>7.92434821050847E-6</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>21</v>
@@ -513,7 +510,7 @@
         <v>32.0</v>
       </c>
       <c r="F12" t="n" s="7">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G12" t="s" s="4">
         <v>11</v>
@@ -524,22 +521,22 @@
     </row>
     <row r="13" outlineLevel="1">
       <c r="A13" t="n" s="5">
-        <v>1.5622066712239757E-5</v>
+        <v>7.206521786429221E-6</v>
       </c>
       <c r="B13" t="s" s="4">
         <v>22</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>11.30434799194336</v>
+        <v>10.8695650100708</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>5.65217399597168</v>
+        <v>60.71390914916992</v>
       </c>
       <c r="E13" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F13" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G13" t="s" s="4">
         <v>11</v>
@@ -550,59 +547,59 @@
     </row>
     <row r="14" outlineLevel="1">
       <c r="A14" t="n" s="5">
-        <v>1.548282671137713E-5</v>
+        <v>6.816521818109322E-6</v>
       </c>
       <c r="B14" t="s" s="4">
         <v>23</v>
       </c>
       <c r="C14" t="n" s="2">
-        <v>10.8695650100708</v>
+        <v>11.30434799194336</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>61.279170989990234</v>
+        <v>5.533477783203125</v>
       </c>
       <c r="E14" t="n" s="7">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="F14" t="n" s="7">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G14" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H14" t="s" s="4">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" outlineLevel="1">
       <c r="A15" t="n" s="5">
-        <v>1.5021217222965788E-5</v>
+        <v>6.6358693402435165E-6</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="n" s="2">
         <v>10.8695650100708</v>
       </c>
       <c r="D15" t="n" s="2">
-        <v>60.71390914916992</v>
+        <v>61.279170989990234</v>
       </c>
       <c r="E15" t="n" s="7">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
       <c r="F15" t="n" s="7">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G15" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H15" t="s" s="4">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" outlineLevel="1">
       <c r="A16" t="n" s="5">
-        <v>9.648083505453542E-6</v>
+        <v>6.203478278621333E-6</v>
       </c>
       <c r="B16" t="s" s="4">
         <v>26</v>
@@ -617,7 +614,7 @@
         <v>18.0</v>
       </c>
       <c r="F16" t="n" s="7">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="G16" t="s" s="4">
         <v>11</v>
@@ -628,7 +625,7 @@
     </row>
     <row r="17" outlineLevel="1">
       <c r="A17" t="n" s="5">
-        <v>7.80877144279657E-6</v>
+        <v>5.309782409312902E-6</v>
       </c>
       <c r="B17" t="s" s="4">
         <v>28</v>
@@ -643,18 +640,18 @@
         <v>12.0</v>
       </c>
       <c r="F17" t="n" s="7">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G17" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H17" t="s" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" outlineLevel="1">
       <c r="A18" t="n" s="5">
-        <v>2.99144039672683E-6</v>
+        <v>3.3532608085806714E-6</v>
       </c>
       <c r="B18" t="s" s="4">
         <v>29</v>
@@ -663,122 +660,96 @@
         <v>10.8695650100708</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>62.10765075683594</v>
+        <v>56.80443572998047</v>
       </c>
       <c r="E18" t="n" s="7">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="F18" t="n" s="7">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="G18" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H18" t="s" s="4">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" outlineLevel="1">
       <c r="A19" t="n" s="5">
-        <v>1.9158521809004014E-6</v>
+        <v>2.0815216430492E-6</v>
       </c>
       <c r="B19" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="C19" t="n" s="2">
+        <v>10.8695650100708</v>
+      </c>
+      <c r="D19" t="n" s="2">
+        <v>67.27208709716797</v>
+      </c>
+      <c r="E19" t="n" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="F19" t="n" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="G19" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s" s="4">
         <v>30</v>
-      </c>
-      <c r="C19" t="n" s="2">
-        <v>11.30434799194336</v>
-      </c>
-      <c r="D19" t="n" s="2">
-        <v>55.85365295410156</v>
-      </c>
-      <c r="E19" t="n" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="F19" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G19" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s" s="4">
-        <v>12</v>
       </c>
     </row>
     <row r="20" outlineLevel="1">
       <c r="A20" t="n" s="5">
-        <v>1.3629311297336244E-6</v>
+        <v>1.1249999261053745E-6</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" t="n" s="2">
         <v>10.8695650100708</v>
       </c>
       <c r="D20" t="n" s="2">
-        <v>67.27208709716797</v>
+        <v>62.10765075683594</v>
       </c>
       <c r="E20" t="n" s="7">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="F20" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G20" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H20" t="s" s="4">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" outlineLevel="1">
       <c r="A21" t="n" s="5">
-        <v>1.3629311297336244E-6</v>
+        <v>5.765217565567582E-7</v>
       </c>
       <c r="B21" t="s" s="4">
         <v>33</v>
       </c>
       <c r="C21" t="n" s="2">
-        <v>10.8695650100708</v>
+        <v>11.30434799194336</v>
       </c>
       <c r="D21" t="n" s="2">
-        <v>56.80443572998047</v>
+        <v>55.85365295410156</v>
       </c>
       <c r="E21" t="n" s="7">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F21" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G21" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H21" t="s" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" outlineLevel="1">
-      <c r="A22" t="n" s="5">
-        <v>7.229010634546285E-7</v>
-      </c>
-      <c r="B22" t="s" s="4">
-        <v>34</v>
-      </c>
-      <c r="C22" t="n" s="2">
-        <v>10.8695650100708</v>
-      </c>
-      <c r="D22" t="n" s="2">
-        <v>62.11869812011719</v>
-      </c>
-      <c r="E22" t="n" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F22" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G22" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s" s="4">
         <v>12</v>
       </c>
     </row>

</xml_diff>